<commit_message>
classifica teste até tweet n100
</commit_message>
<xml_diff>
--- a/SPTrans.xlsx
+++ b/SPTrans.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crazy\Documents\Projetos\P2_CD19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FE555B-7DFA-4BB0-99A0-CA30F2348D07}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A834ABD-4247-4580-92F9-2ADE99237AC8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
     <sheet name="Teste" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="503">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1687,6 +1688,9 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>Classificacao</t>
   </si>
 </sst>
 </file>
@@ -1745,11 +1749,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2096,22 +2097,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
-      <selection activeCell="B301" sqref="B301"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.46484375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="2" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -2119,7 +2124,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -2127,7 +2132,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -2135,7 +2140,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -2143,7 +2148,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -2151,7 +2156,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -2159,7 +2164,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -2167,7 +2172,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -2175,7 +2180,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -2183,7 +2188,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -2191,7 +2196,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="285" x14ac:dyDescent="0.45">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -2199,7 +2204,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -2207,7 +2212,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -2215,7 +2220,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -2223,7 +2228,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
@@ -2231,7 +2236,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="356.25" x14ac:dyDescent="0.45">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -2239,7 +2244,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -2247,7 +2252,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
@@ -2255,7 +2260,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="228" x14ac:dyDescent="0.45">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -2263,7 +2268,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="114" x14ac:dyDescent="0.45">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -2271,7 +2276,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -2279,7 +2284,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -2287,7 +2292,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B24" t="s">
@@ -2295,7 +2300,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B25" t="s">
@@ -2303,7 +2308,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="342" x14ac:dyDescent="0.45">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B26" t="s">
@@ -2311,7 +2316,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
@@ -2319,7 +2324,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
@@ -2327,7 +2332,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B29" t="s">
@@ -2335,7 +2340,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B30" t="s">
@@ -2343,7 +2348,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B31" t="s">
@@ -2351,7 +2356,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
@@ -2359,7 +2364,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
@@ -2367,7 +2372,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
@@ -2375,7 +2380,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B35" t="s">
@@ -2383,7 +2388,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
@@ -2391,7 +2396,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B37" t="s">
@@ -2399,7 +2404,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="228" x14ac:dyDescent="0.45">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B38" t="s">
@@ -2407,7 +2412,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="285" x14ac:dyDescent="0.45">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B39" t="s">
@@ -2415,7 +2420,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B40" t="s">
@@ -2423,7 +2428,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="228" x14ac:dyDescent="0.45">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B41" t="s">
@@ -2431,7 +2436,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B42" t="s">
@@ -2439,7 +2444,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="285" x14ac:dyDescent="0.45">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B43" t="s">
@@ -2447,7 +2452,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B44" t="s">
@@ -2455,7 +2460,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B45" t="s">
@@ -2463,7 +2468,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="114" x14ac:dyDescent="0.45">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B46" t="s">
@@ -2471,7 +2476,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B47" t="s">
@@ -2479,7 +2484,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B48" t="s">
@@ -2487,7 +2492,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B49" t="s">
@@ -2495,7 +2500,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B50" t="s">
@@ -2503,7 +2508,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="342" x14ac:dyDescent="0.45">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B51" t="s">
@@ -2511,7 +2516,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B52" t="s">
@@ -2519,7 +2524,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B53" t="s">
@@ -2527,7 +2532,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B54" t="s">
@@ -2535,7 +2540,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B55" t="s">
@@ -2543,7 +2548,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B56" t="s">
@@ -2551,7 +2556,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B57" t="s">
@@ -2559,7 +2564,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B58" t="s">
@@ -2567,7 +2572,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B59" t="s">
@@ -2575,7 +2580,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" ht="114" x14ac:dyDescent="0.45">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B60" t="s">
@@ -2583,7 +2588,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B61" t="s">
@@ -2591,7 +2596,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="114" x14ac:dyDescent="0.45">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B62" t="s">
@@ -2599,7 +2604,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" ht="285" x14ac:dyDescent="0.45">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B63" t="s">
@@ -2607,7 +2612,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B64" t="s">
@@ -2615,7 +2620,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B65" t="s">
@@ -2623,7 +2628,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B66" t="s">
@@ -2631,7 +2636,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B67" t="s">
@@ -2639,7 +2644,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="242.25" x14ac:dyDescent="0.45">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B68" t="s">
@@ -2647,7 +2652,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B69" t="s">
@@ -2655,7 +2660,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" ht="114" x14ac:dyDescent="0.45">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B70" t="s">
@@ -2663,7 +2668,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B71" t="s">
@@ -2671,7 +2676,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" ht="228" x14ac:dyDescent="0.45">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B72" t="s">
@@ -2679,7 +2684,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B73" t="s">
@@ -2687,7 +2692,7 @@
       </c>
     </row>
     <row r="74" spans="1:2" ht="228" x14ac:dyDescent="0.45">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B74" t="s">
@@ -2695,7 +2700,7 @@
       </c>
     </row>
     <row r="75" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B75" t="s">
@@ -2703,7 +2708,7 @@
       </c>
     </row>
     <row r="76" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B76" t="s">
@@ -2711,7 +2716,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B77" t="s">
@@ -2719,7 +2724,7 @@
       </c>
     </row>
     <row r="78" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B78" t="s">
@@ -2727,7 +2732,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B79" t="s">
@@ -2735,7 +2740,7 @@
       </c>
     </row>
     <row r="80" spans="1:2" ht="285" x14ac:dyDescent="0.45">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B80" t="s">
@@ -2743,7 +2748,7 @@
       </c>
     </row>
     <row r="81" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B81" t="s">
@@ -2751,7 +2756,7 @@
       </c>
     </row>
     <row r="82" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B82" t="s">
@@ -2759,7 +2764,7 @@
       </c>
     </row>
     <row r="83" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B83" t="s">
@@ -2767,7 +2772,7 @@
       </c>
     </row>
     <row r="84" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B84" t="s">
@@ -2775,7 +2780,7 @@
       </c>
     </row>
     <row r="85" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B85" t="s">
@@ -2783,7 +2788,7 @@
       </c>
     </row>
     <row r="86" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B86" t="s">
@@ -2791,7 +2796,7 @@
       </c>
     </row>
     <row r="87" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B87" t="s">
@@ -2799,7 +2804,7 @@
       </c>
     </row>
     <row r="88" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B88" t="s">
@@ -2807,7 +2812,7 @@
       </c>
     </row>
     <row r="89" spans="1:2" ht="342" x14ac:dyDescent="0.45">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B89" t="s">
@@ -2815,7 +2820,7 @@
       </c>
     </row>
     <row r="90" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B90" t="s">
@@ -2823,7 +2828,7 @@
       </c>
     </row>
     <row r="91" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B91" t="s">
@@ -2831,7 +2836,7 @@
       </c>
     </row>
     <row r="92" spans="1:2" ht="356.25" x14ac:dyDescent="0.45">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B92" t="s">
@@ -2839,7 +2844,7 @@
       </c>
     </row>
     <row r="93" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B93" t="s">
@@ -2847,7 +2852,7 @@
       </c>
     </row>
     <row r="94" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B94" t="s">
@@ -2855,7 +2860,7 @@
       </c>
     </row>
     <row r="95" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B95" t="s">
@@ -2863,7 +2868,7 @@
       </c>
     </row>
     <row r="96" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B96" t="s">
@@ -2871,7 +2876,7 @@
       </c>
     </row>
     <row r="97" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B97" t="s">
@@ -2879,7 +2884,7 @@
       </c>
     </row>
     <row r="98" spans="1:2" ht="384.75" x14ac:dyDescent="0.45">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B98" t="s">
@@ -2887,7 +2892,7 @@
       </c>
     </row>
     <row r="99" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B99" t="s">
@@ -2895,7 +2900,7 @@
       </c>
     </row>
     <row r="100" spans="1:2" ht="342" x14ac:dyDescent="0.45">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B100" t="s">
@@ -2903,7 +2908,7 @@
       </c>
     </row>
     <row r="101" spans="1:2" ht="285" x14ac:dyDescent="0.45">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B101" t="s">
@@ -2911,7 +2916,7 @@
       </c>
     </row>
     <row r="102" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B102" t="s">
@@ -2919,7 +2924,7 @@
       </c>
     </row>
     <row r="103" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B103" t="s">
@@ -2927,7 +2932,7 @@
       </c>
     </row>
     <row r="104" spans="1:2" ht="342" x14ac:dyDescent="0.45">
-      <c r="A104" s="3" t="s">
+      <c r="A104" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B104" t="s">
@@ -2935,7 +2940,7 @@
       </c>
     </row>
     <row r="105" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B105" t="s">
@@ -2943,7 +2948,7 @@
       </c>
     </row>
     <row r="106" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A106" s="3" t="s">
+      <c r="A106" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B106" t="s">
@@ -2951,7 +2956,7 @@
       </c>
     </row>
     <row r="107" spans="1:2" ht="342" x14ac:dyDescent="0.45">
-      <c r="A107" s="3" t="s">
+      <c r="A107" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B107" t="s">
@@ -2959,7 +2964,7 @@
       </c>
     </row>
     <row r="108" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B108" t="s">
@@ -2967,7 +2972,7 @@
       </c>
     </row>
     <row r="109" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B109" t="s">
@@ -2975,7 +2980,7 @@
       </c>
     </row>
     <row r="110" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="A110" s="3" t="s">
+      <c r="A110" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B110" t="s">
@@ -2983,7 +2988,7 @@
       </c>
     </row>
     <row r="111" spans="1:2" ht="228" x14ac:dyDescent="0.45">
-      <c r="A111" s="3" t="s">
+      <c r="A111" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B111" t="s">
@@ -2991,7 +2996,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" ht="114" x14ac:dyDescent="0.45">
-      <c r="A112" s="3" t="s">
+      <c r="A112" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B112" t="s">
@@ -2999,7 +3004,7 @@
       </c>
     </row>
     <row r="113" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B113" t="s">
@@ -3007,7 +3012,7 @@
       </c>
     </row>
     <row r="114" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A114" s="3" t="s">
+      <c r="A114" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B114" t="s">
@@ -3015,7 +3020,7 @@
       </c>
     </row>
     <row r="115" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A115" s="3" t="s">
+      <c r="A115" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B115" t="s">
@@ -3023,7 +3028,7 @@
       </c>
     </row>
     <row r="116" spans="1:2" ht="228" x14ac:dyDescent="0.45">
-      <c r="A116" s="3" t="s">
+      <c r="A116" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B116" t="s">
@@ -3031,7 +3036,7 @@
       </c>
     </row>
     <row r="117" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A117" s="3" t="s">
+      <c r="A117" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B117" t="s">
@@ -3039,7 +3044,7 @@
       </c>
     </row>
     <row r="118" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A118" s="3" t="s">
+      <c r="A118" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B118" t="s">
@@ -3047,7 +3052,7 @@
       </c>
     </row>
     <row r="119" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A119" s="3" t="s">
+      <c r="A119" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B119" t="s">
@@ -3055,7 +3060,7 @@
       </c>
     </row>
     <row r="120" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A120" s="3" t="s">
+      <c r="A120" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B120" t="s">
@@ -3063,7 +3068,7 @@
       </c>
     </row>
     <row r="121" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A121" s="3" t="s">
+      <c r="A121" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B121" t="s">
@@ -3071,7 +3076,7 @@
       </c>
     </row>
     <row r="122" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A122" s="3" t="s">
+      <c r="A122" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B122" t="s">
@@ -3079,7 +3084,7 @@
       </c>
     </row>
     <row r="123" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A123" s="3" t="s">
+      <c r="A123" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B123" t="s">
@@ -3087,7 +3092,7 @@
       </c>
     </row>
     <row r="124" spans="1:2" ht="114" x14ac:dyDescent="0.45">
-      <c r="A124" s="3" t="s">
+      <c r="A124" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B124" t="s">
@@ -3095,7 +3100,7 @@
       </c>
     </row>
     <row r="125" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
-      <c r="A125" s="3" t="s">
+      <c r="A125" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B125" t="s">
@@ -3103,7 +3108,7 @@
       </c>
     </row>
     <row r="126" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A126" s="3" t="s">
+      <c r="A126" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B126" t="s">
@@ -3111,7 +3116,7 @@
       </c>
     </row>
     <row r="127" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A127" s="3" t="s">
+      <c r="A127" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B127" t="s">
@@ -3119,7 +3124,7 @@
       </c>
     </row>
     <row r="128" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A128" s="3" t="s">
+      <c r="A128" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B128" t="s">
@@ -3127,7 +3132,7 @@
       </c>
     </row>
     <row r="129" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A129" s="3" t="s">
+      <c r="A129" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B129" t="s">
@@ -3135,7 +3140,7 @@
       </c>
     </row>
     <row r="130" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A130" s="3" t="s">
+      <c r="A130" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B130" t="s">
@@ -3143,7 +3148,7 @@
       </c>
     </row>
     <row r="131" spans="1:2" ht="370.5" x14ac:dyDescent="0.45">
-      <c r="A131" s="3" t="s">
+      <c r="A131" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B131" t="s">
@@ -3151,7 +3156,7 @@
       </c>
     </row>
     <row r="132" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A132" s="3" t="s">
+      <c r="A132" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B132" t="s">
@@ -3159,7 +3164,7 @@
       </c>
     </row>
     <row r="133" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A133" s="3" t="s">
+      <c r="A133" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B133" t="s">
@@ -3167,7 +3172,7 @@
       </c>
     </row>
     <row r="134" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A134" s="3" t="s">
+      <c r="A134" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B134" t="s">
@@ -3175,7 +3180,7 @@
       </c>
     </row>
     <row r="135" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A135" s="3" t="s">
+      <c r="A135" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B135" t="s">
@@ -3183,7 +3188,7 @@
       </c>
     </row>
     <row r="136" spans="1:2" ht="114" x14ac:dyDescent="0.45">
-      <c r="A136" s="3" t="s">
+      <c r="A136" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B136" t="s">
@@ -3191,7 +3196,7 @@
       </c>
     </row>
     <row r="137" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A137" s="3" t="s">
+      <c r="A137" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B137" t="s">
@@ -3199,7 +3204,7 @@
       </c>
     </row>
     <row r="138" spans="1:2" ht="114" x14ac:dyDescent="0.45">
-      <c r="A138" s="3" t="s">
+      <c r="A138" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B138" t="s">
@@ -3207,7 +3212,7 @@
       </c>
     </row>
     <row r="139" spans="1:2" ht="356.25" x14ac:dyDescent="0.45">
-      <c r="A139" s="3" t="s">
+      <c r="A139" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B139" t="s">
@@ -3215,7 +3220,7 @@
       </c>
     </row>
     <row r="140" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A140" s="3" t="s">
+      <c r="A140" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B140" t="s">
@@ -3223,7 +3228,7 @@
       </c>
     </row>
     <row r="141" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A141" s="3" t="s">
+      <c r="A141" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B141" t="s">
@@ -3231,7 +3236,7 @@
       </c>
     </row>
     <row r="142" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
-      <c r="A142" s="3" t="s">
+      <c r="A142" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B142" t="s">
@@ -3239,7 +3244,7 @@
       </c>
     </row>
     <row r="143" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A143" s="3" t="s">
+      <c r="A143" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B143" t="s">
@@ -3247,7 +3252,7 @@
       </c>
     </row>
     <row r="144" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A144" s="3" t="s">
+      <c r="A144" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B144" t="s">
@@ -3255,7 +3260,7 @@
       </c>
     </row>
     <row r="145" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="A145" s="3" t="s">
+      <c r="A145" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B145" t="s">
@@ -3263,7 +3268,7 @@
       </c>
     </row>
     <row r="146" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A146" s="3" t="s">
+      <c r="A146" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B146" t="s">
@@ -3271,7 +3276,7 @@
       </c>
     </row>
     <row r="147" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A147" s="3" t="s">
+      <c r="A147" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B147" t="s">
@@ -3279,7 +3284,7 @@
       </c>
     </row>
     <row r="148" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A148" s="3" t="s">
+      <c r="A148" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B148" t="s">
@@ -3287,7 +3292,7 @@
       </c>
     </row>
     <row r="149" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A149" s="3" t="s">
+      <c r="A149" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B149" t="s">
@@ -3295,7 +3300,7 @@
       </c>
     </row>
     <row r="150" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
-      <c r="A150" s="3" t="s">
+      <c r="A150" s="2" t="s">
         <v>149</v>
       </c>
       <c r="B150" t="s">
@@ -3303,7 +3308,7 @@
       </c>
     </row>
     <row r="151" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A151" s="3" t="s">
+      <c r="A151" s="2" t="s">
         <v>150</v>
       </c>
       <c r="B151" t="s">
@@ -3311,7 +3316,7 @@
       </c>
     </row>
     <row r="152" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A152" s="3" t="s">
+      <c r="A152" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B152" t="s">
@@ -3319,7 +3324,7 @@
       </c>
     </row>
     <row r="153" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
-      <c r="A153" s="3" t="s">
+      <c r="A153" s="2" t="s">
         <v>152</v>
       </c>
       <c r="B153" t="s">
@@ -3327,7 +3332,7 @@
       </c>
     </row>
     <row r="154" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A154" s="3" t="s">
+      <c r="A154" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B154" t="s">
@@ -3335,7 +3340,7 @@
       </c>
     </row>
     <row r="155" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A155" s="3" t="s">
+      <c r="A155" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B155" t="s">
@@ -3343,7 +3348,7 @@
       </c>
     </row>
     <row r="156" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A156" s="3" t="s">
+      <c r="A156" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B156" t="s">
@@ -3351,7 +3356,7 @@
       </c>
     </row>
     <row r="157" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A157" s="3" t="s">
+      <c r="A157" s="2" t="s">
         <v>156</v>
       </c>
       <c r="B157" t="s">
@@ -3359,7 +3364,7 @@
       </c>
     </row>
     <row r="158" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A158" s="3" t="s">
+      <c r="A158" s="2" t="s">
         <v>157</v>
       </c>
       <c r="B158" t="s">
@@ -3367,7 +3372,7 @@
       </c>
     </row>
     <row r="159" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A159" s="3" t="s">
+      <c r="A159" s="2" t="s">
         <v>158</v>
       </c>
       <c r="B159" t="s">
@@ -3375,7 +3380,7 @@
       </c>
     </row>
     <row r="160" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A160" s="3" t="s">
+      <c r="A160" s="2" t="s">
         <v>159</v>
       </c>
       <c r="B160" t="s">
@@ -3383,7 +3388,7 @@
       </c>
     </row>
     <row r="161" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A161" s="3" t="s">
+      <c r="A161" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B161" t="s">
@@ -3391,7 +3396,7 @@
       </c>
     </row>
     <row r="162" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A162" s="3" t="s">
+      <c r="A162" s="2" t="s">
         <v>161</v>
       </c>
       <c r="B162" t="s">
@@ -3399,7 +3404,7 @@
       </c>
     </row>
     <row r="163" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A163" s="3" t="s">
+      <c r="A163" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B163" t="s">
@@ -3407,7 +3412,7 @@
       </c>
     </row>
     <row r="164" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A164" s="3" t="s">
+      <c r="A164" s="2" t="s">
         <v>163</v>
       </c>
       <c r="B164" t="s">
@@ -3415,7 +3420,7 @@
       </c>
     </row>
     <row r="165" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A165" s="3" t="s">
+      <c r="A165" s="2" t="s">
         <v>164</v>
       </c>
       <c r="B165" t="s">
@@ -3423,7 +3428,7 @@
       </c>
     </row>
     <row r="166" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="A166" s="3" t="s">
+      <c r="A166" s="2" t="s">
         <v>165</v>
       </c>
       <c r="B166" t="s">
@@ -3431,7 +3436,7 @@
       </c>
     </row>
     <row r="167" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
-      <c r="A167" s="3" t="s">
+      <c r="A167" s="2" t="s">
         <v>166</v>
       </c>
       <c r="B167" t="s">
@@ -3439,7 +3444,7 @@
       </c>
     </row>
     <row r="168" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A168" s="3" t="s">
+      <c r="A168" s="2" t="s">
         <v>167</v>
       </c>
       <c r="B168" t="s">
@@ -3447,7 +3452,7 @@
       </c>
     </row>
     <row r="169" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A169" s="3" t="s">
+      <c r="A169" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B169" t="s">
@@ -3455,7 +3460,7 @@
       </c>
     </row>
     <row r="170" spans="1:2" ht="342" x14ac:dyDescent="0.45">
-      <c r="A170" s="3" t="s">
+      <c r="A170" s="2" t="s">
         <v>169</v>
       </c>
       <c r="B170" t="s">
@@ -3463,7 +3468,7 @@
       </c>
     </row>
     <row r="171" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A171" s="3" t="s">
+      <c r="A171" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B171" t="s">
@@ -3471,7 +3476,7 @@
       </c>
     </row>
     <row r="172" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A172" s="3" t="s">
+      <c r="A172" s="2" t="s">
         <v>171</v>
       </c>
       <c r="B172" t="s">
@@ -3479,7 +3484,7 @@
       </c>
     </row>
     <row r="173" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A173" s="3" t="s">
+      <c r="A173" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B173" t="s">
@@ -3487,7 +3492,7 @@
       </c>
     </row>
     <row r="174" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A174" s="3" t="s">
+      <c r="A174" s="2" t="s">
         <v>173</v>
       </c>
       <c r="B174" t="s">
@@ -3495,7 +3500,7 @@
       </c>
     </row>
     <row r="175" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A175" s="3" t="s">
+      <c r="A175" s="2" t="s">
         <v>174</v>
       </c>
       <c r="B175" t="s">
@@ -3503,7 +3508,7 @@
       </c>
     </row>
     <row r="176" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="A176" s="3" t="s">
+      <c r="A176" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B176" t="s">
@@ -3511,7 +3516,7 @@
       </c>
     </row>
     <row r="177" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A177" s="3" t="s">
+      <c r="A177" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B177" t="s">
@@ -3519,7 +3524,7 @@
       </c>
     </row>
     <row r="178" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
-      <c r="A178" s="3" t="s">
+      <c r="A178" s="2" t="s">
         <v>177</v>
       </c>
       <c r="B178" t="s">
@@ -3527,7 +3532,7 @@
       </c>
     </row>
     <row r="179" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A179" s="3" t="s">
+      <c r="A179" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B179" t="s">
@@ -3535,7 +3540,7 @@
       </c>
     </row>
     <row r="180" spans="1:2" ht="370.5" x14ac:dyDescent="0.45">
-      <c r="A180" s="3" t="s">
+      <c r="A180" s="2" t="s">
         <v>179</v>
       </c>
       <c r="B180" t="s">
@@ -3543,7 +3548,7 @@
       </c>
     </row>
     <row r="181" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A181" s="3" t="s">
+      <c r="A181" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B181" t="s">
@@ -3551,7 +3556,7 @@
       </c>
     </row>
     <row r="182" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A182" s="3" t="s">
+      <c r="A182" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B182" t="s">
@@ -3559,7 +3564,7 @@
       </c>
     </row>
     <row r="183" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A183" s="3" t="s">
+      <c r="A183" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B183" t="s">
@@ -3567,7 +3572,7 @@
       </c>
     </row>
     <row r="184" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A184" s="3" t="s">
+      <c r="A184" s="2" t="s">
         <v>183</v>
       </c>
       <c r="B184" t="s">
@@ -3575,7 +3580,7 @@
       </c>
     </row>
     <row r="185" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A185" s="3" t="s">
+      <c r="A185" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B185" t="s">
@@ -3583,7 +3588,7 @@
       </c>
     </row>
     <row r="186" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A186" s="3" t="s">
+      <c r="A186" s="2" t="s">
         <v>185</v>
       </c>
       <c r="B186" t="s">
@@ -3591,7 +3596,7 @@
       </c>
     </row>
     <row r="187" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A187" s="3" t="s">
+      <c r="A187" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B187" t="s">
@@ -3599,7 +3604,7 @@
       </c>
     </row>
     <row r="188" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A188" s="3" t="s">
+      <c r="A188" s="2" t="s">
         <v>187</v>
       </c>
       <c r="B188" t="s">
@@ -3607,7 +3612,7 @@
       </c>
     </row>
     <row r="189" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A189" s="3" t="s">
+      <c r="A189" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B189" t="s">
@@ -3615,7 +3620,7 @@
       </c>
     </row>
     <row r="190" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A190" s="3" t="s">
+      <c r="A190" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B190" t="s">
@@ -3623,7 +3628,7 @@
       </c>
     </row>
     <row r="191" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A191" s="3" t="s">
+      <c r="A191" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B191" t="s">
@@ -3631,7 +3636,7 @@
       </c>
     </row>
     <row r="192" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A192" s="3" t="s">
+      <c r="A192" s="2" t="s">
         <v>191</v>
       </c>
       <c r="B192" t="s">
@@ -3639,7 +3644,7 @@
       </c>
     </row>
     <row r="193" spans="1:2" ht="242.25" x14ac:dyDescent="0.45">
-      <c r="A193" s="3" t="s">
+      <c r="A193" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B193" t="s">
@@ -3647,7 +3652,7 @@
       </c>
     </row>
     <row r="194" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A194" s="3" t="s">
+      <c r="A194" s="2" t="s">
         <v>193</v>
       </c>
       <c r="B194" t="s">
@@ -3655,7 +3660,7 @@
       </c>
     </row>
     <row r="195" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A195" s="3" t="s">
+      <c r="A195" s="2" t="s">
         <v>194</v>
       </c>
       <c r="B195" t="s">
@@ -3663,7 +3668,7 @@
       </c>
     </row>
     <row r="196" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A196" s="3" t="s">
+      <c r="A196" s="2" t="s">
         <v>195</v>
       </c>
       <c r="B196" t="s">
@@ -3671,7 +3676,7 @@
       </c>
     </row>
     <row r="197" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A197" s="3" t="s">
+      <c r="A197" s="2" t="s">
         <v>196</v>
       </c>
       <c r="B197" t="s">
@@ -3679,7 +3684,7 @@
       </c>
     </row>
     <row r="198" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A198" s="3" t="s">
+      <c r="A198" s="2" t="s">
         <v>197</v>
       </c>
       <c r="B198" t="s">
@@ -3687,7 +3692,7 @@
       </c>
     </row>
     <row r="199" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A199" s="3" t="s">
+      <c r="A199" s="2" t="s">
         <v>198</v>
       </c>
       <c r="B199" t="s">
@@ -3695,7 +3700,7 @@
       </c>
     </row>
     <row r="200" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A200" s="3" t="s">
+      <c r="A200" s="2" t="s">
         <v>199</v>
       </c>
       <c r="B200" t="s">
@@ -3703,7 +3708,7 @@
       </c>
     </row>
     <row r="201" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
-      <c r="A201" s="3" t="s">
+      <c r="A201" s="2" t="s">
         <v>200</v>
       </c>
       <c r="B201" t="s">
@@ -3711,7 +3716,7 @@
       </c>
     </row>
     <row r="202" spans="1:2" ht="114" x14ac:dyDescent="0.45">
-      <c r="A202" s="3" t="s">
+      <c r="A202" s="2" t="s">
         <v>201</v>
       </c>
       <c r="B202" t="s">
@@ -3719,7 +3724,7 @@
       </c>
     </row>
     <row r="203" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A203" s="3" t="s">
+      <c r="A203" s="2" t="s">
         <v>202</v>
       </c>
       <c r="B203" t="s">
@@ -3727,7 +3732,7 @@
       </c>
     </row>
     <row r="204" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
-      <c r="A204" s="3" t="s">
+      <c r="A204" s="2" t="s">
         <v>203</v>
       </c>
       <c r="B204" t="s">
@@ -3735,7 +3740,7 @@
       </c>
     </row>
     <row r="205" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A205" s="3" t="s">
+      <c r="A205" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B205" t="s">
@@ -3743,7 +3748,7 @@
       </c>
     </row>
     <row r="206" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A206" s="3" t="s">
+      <c r="A206" s="2" t="s">
         <v>205</v>
       </c>
       <c r="B206" t="s">
@@ -3751,12 +3756,12 @@
       </c>
     </row>
     <row r="207" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A207" s="3" t="s">
+      <c r="A207" s="2" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A208" s="3" t="s">
+      <c r="A208" s="2" t="s">
         <v>207</v>
       </c>
       <c r="B208" t="s">
@@ -3764,7 +3769,7 @@
       </c>
     </row>
     <row r="209" spans="1:2" ht="242.25" x14ac:dyDescent="0.45">
-      <c r="A209" s="3" t="s">
+      <c r="A209" s="2" t="s">
         <v>208</v>
       </c>
       <c r="B209" t="s">
@@ -3772,7 +3777,7 @@
       </c>
     </row>
     <row r="210" spans="1:2" ht="342" x14ac:dyDescent="0.45">
-      <c r="A210" s="3" t="s">
+      <c r="A210" s="2" t="s">
         <v>209</v>
       </c>
       <c r="B210" t="s">
@@ -3780,7 +3785,7 @@
       </c>
     </row>
     <row r="211" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
-      <c r="A211" s="3" t="s">
+      <c r="A211" s="2" t="s">
         <v>210</v>
       </c>
       <c r="B211" t="s">
@@ -3788,7 +3793,7 @@
       </c>
     </row>
     <row r="212" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A212" s="3" t="s">
+      <c r="A212" s="2" t="s">
         <v>211</v>
       </c>
       <c r="B212" t="s">
@@ -3796,7 +3801,7 @@
       </c>
     </row>
     <row r="213" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A213" s="3" t="s">
+      <c r="A213" s="2" t="s">
         <v>212</v>
       </c>
       <c r="B213" t="s">
@@ -3804,7 +3809,7 @@
       </c>
     </row>
     <row r="214" spans="1:2" ht="242.25" x14ac:dyDescent="0.45">
-      <c r="A214" s="3" t="s">
+      <c r="A214" s="2" t="s">
         <v>213</v>
       </c>
       <c r="B214" t="s">
@@ -3812,7 +3817,7 @@
       </c>
     </row>
     <row r="215" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A215" s="3" t="s">
+      <c r="A215" s="2" t="s">
         <v>214</v>
       </c>
       <c r="B215" t="s">
@@ -3820,7 +3825,7 @@
       </c>
     </row>
     <row r="216" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
-      <c r="A216" s="3" t="s">
+      <c r="A216" s="2" t="s">
         <v>215</v>
       </c>
       <c r="B216" t="s">
@@ -3828,7 +3833,7 @@
       </c>
     </row>
     <row r="217" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A217" s="3" t="s">
+      <c r="A217" s="2" t="s">
         <v>216</v>
       </c>
       <c r="B217" t="s">
@@ -3836,7 +3841,7 @@
       </c>
     </row>
     <row r="218" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A218" s="3" t="s">
+      <c r="A218" s="2" t="s">
         <v>217</v>
       </c>
       <c r="B218" t="s">
@@ -3844,7 +3849,7 @@
       </c>
     </row>
     <row r="219" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A219" s="3" t="s">
+      <c r="A219" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B219" t="s">
@@ -3852,7 +3857,7 @@
       </c>
     </row>
     <row r="220" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A220" s="3" t="s">
+      <c r="A220" s="2" t="s">
         <v>219</v>
       </c>
       <c r="B220" t="s">
@@ -3860,7 +3865,7 @@
       </c>
     </row>
     <row r="221" spans="1:2" ht="342" x14ac:dyDescent="0.45">
-      <c r="A221" s="3" t="s">
+      <c r="A221" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B221" t="s">
@@ -3868,7 +3873,7 @@
       </c>
     </row>
     <row r="222" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A222" s="3" t="s">
+      <c r="A222" s="2" t="s">
         <v>221</v>
       </c>
       <c r="B222" t="s">
@@ -3876,7 +3881,7 @@
       </c>
     </row>
     <row r="223" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A223" s="3" t="s">
+      <c r="A223" s="2" t="s">
         <v>222</v>
       </c>
       <c r="B223" t="s">
@@ -3884,7 +3889,7 @@
       </c>
     </row>
     <row r="224" spans="1:2" ht="114" x14ac:dyDescent="0.45">
-      <c r="A224" s="3" t="s">
+      <c r="A224" s="2" t="s">
         <v>223</v>
       </c>
       <c r="B224" t="s">
@@ -3892,7 +3897,7 @@
       </c>
     </row>
     <row r="225" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A225" s="3" t="s">
+      <c r="A225" s="2" t="s">
         <v>224</v>
       </c>
       <c r="B225" t="s">
@@ -3900,7 +3905,7 @@
       </c>
     </row>
     <row r="226" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A226" s="3" t="s">
+      <c r="A226" s="2" t="s">
         <v>225</v>
       </c>
       <c r="B226" t="s">
@@ -3908,7 +3913,7 @@
       </c>
     </row>
     <row r="227" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A227" s="3" t="s">
+      <c r="A227" s="2" t="s">
         <v>226</v>
       </c>
       <c r="B227" t="s">
@@ -3916,7 +3921,7 @@
       </c>
     </row>
     <row r="228" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A228" s="3" t="s">
+      <c r="A228" s="2" t="s">
         <v>227</v>
       </c>
       <c r="B228" t="s">
@@ -3924,7 +3929,7 @@
       </c>
     </row>
     <row r="229" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A229" s="3" t="s">
+      <c r="A229" s="2" t="s">
         <v>228</v>
       </c>
       <c r="B229" t="s">
@@ -3932,7 +3937,7 @@
       </c>
     </row>
     <row r="230" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A230" s="3" t="s">
+      <c r="A230" s="2" t="s">
         <v>229</v>
       </c>
       <c r="B230" t="s">
@@ -3940,7 +3945,7 @@
       </c>
     </row>
     <row r="231" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A231" s="3" t="s">
+      <c r="A231" s="2" t="s">
         <v>230</v>
       </c>
       <c r="B231" t="s">
@@ -3948,7 +3953,7 @@
       </c>
     </row>
     <row r="232" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A232" s="3" t="s">
+      <c r="A232" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B232" t="s">
@@ -3956,7 +3961,7 @@
       </c>
     </row>
     <row r="233" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A233" s="3" t="s">
+      <c r="A233" s="2" t="s">
         <v>232</v>
       </c>
       <c r="B233" t="s">
@@ -3964,7 +3969,7 @@
       </c>
     </row>
     <row r="234" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A234" s="3" t="s">
+      <c r="A234" s="2" t="s">
         <v>233</v>
       </c>
       <c r="B234" t="s">
@@ -3972,7 +3977,7 @@
       </c>
     </row>
     <row r="235" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A235" s="3" t="s">
+      <c r="A235" s="2" t="s">
         <v>234</v>
       </c>
       <c r="B235" t="s">
@@ -3980,7 +3985,7 @@
       </c>
     </row>
     <row r="236" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A236" s="3" t="s">
+      <c r="A236" s="2" t="s">
         <v>235</v>
       </c>
       <c r="B236" t="s">
@@ -3988,7 +3993,7 @@
       </c>
     </row>
     <row r="237" spans="1:2" ht="242.25" x14ac:dyDescent="0.45">
-      <c r="A237" s="3" t="s">
+      <c r="A237" s="2" t="s">
         <v>236</v>
       </c>
       <c r="B237" t="s">
@@ -3996,7 +4001,7 @@
       </c>
     </row>
     <row r="238" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A238" s="3" t="s">
+      <c r="A238" s="2" t="s">
         <v>237</v>
       </c>
       <c r="B238" t="s">
@@ -4004,7 +4009,7 @@
       </c>
     </row>
     <row r="239" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A239" s="3" t="s">
+      <c r="A239" s="2" t="s">
         <v>238</v>
       </c>
       <c r="B239" t="s">
@@ -4012,7 +4017,7 @@
       </c>
     </row>
     <row r="240" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A240" s="3" t="s">
+      <c r="A240" s="2" t="s">
         <v>239</v>
       </c>
       <c r="B240" t="s">
@@ -4020,7 +4025,7 @@
       </c>
     </row>
     <row r="241" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A241" s="3" t="s">
+      <c r="A241" s="2" t="s">
         <v>240</v>
       </c>
       <c r="B241" t="s">
@@ -4028,7 +4033,7 @@
       </c>
     </row>
     <row r="242" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A242" s="3" t="s">
+      <c r="A242" s="2" t="s">
         <v>241</v>
       </c>
       <c r="B242" t="s">
@@ -4036,7 +4041,7 @@
       </c>
     </row>
     <row r="243" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A243" s="3" t="s">
+      <c r="A243" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B243" t="s">
@@ -4044,7 +4049,7 @@
       </c>
     </row>
     <row r="244" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A244" s="3" t="s">
+      <c r="A244" s="2" t="s">
         <v>243</v>
       </c>
       <c r="B244" t="s">
@@ -4052,7 +4057,7 @@
       </c>
     </row>
     <row r="245" spans="1:2" ht="114" x14ac:dyDescent="0.45">
-      <c r="A245" s="3" t="s">
+      <c r="A245" s="2" t="s">
         <v>244</v>
       </c>
       <c r="B245" t="s">
@@ -4060,7 +4065,7 @@
       </c>
     </row>
     <row r="246" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A246" s="3" t="s">
+      <c r="A246" s="2" t="s">
         <v>245</v>
       </c>
       <c r="B246" t="s">
@@ -4068,7 +4073,7 @@
       </c>
     </row>
     <row r="247" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A247" s="3" t="s">
+      <c r="A247" s="2" t="s">
         <v>246</v>
       </c>
       <c r="B247" t="s">
@@ -4076,7 +4081,7 @@
       </c>
     </row>
     <row r="248" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A248" s="3" t="s">
+      <c r="A248" s="2" t="s">
         <v>247</v>
       </c>
       <c r="B248" t="s">
@@ -4084,7 +4089,7 @@
       </c>
     </row>
     <row r="249" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A249" s="3" t="s">
+      <c r="A249" s="2" t="s">
         <v>248</v>
       </c>
       <c r="B249" t="s">
@@ -4092,7 +4097,7 @@
       </c>
     </row>
     <row r="250" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A250" s="3" t="s">
+      <c r="A250" s="2" t="s">
         <v>249</v>
       </c>
       <c r="B250" t="s">
@@ -4100,7 +4105,7 @@
       </c>
     </row>
     <row r="251" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
-      <c r="A251" s="3" t="s">
+      <c r="A251" s="2" t="s">
         <v>250</v>
       </c>
       <c r="B251" t="s">
@@ -4108,7 +4113,7 @@
       </c>
     </row>
     <row r="252" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="A252" s="3" t="s">
+      <c r="A252" s="2" t="s">
         <v>251</v>
       </c>
       <c r="B252" t="s">
@@ -4116,7 +4121,7 @@
       </c>
     </row>
     <row r="253" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
-      <c r="A253" s="3" t="s">
+      <c r="A253" s="2" t="s">
         <v>252</v>
       </c>
       <c r="B253" t="s">
@@ -4124,7 +4129,7 @@
       </c>
     </row>
     <row r="254" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A254" s="3" t="s">
+      <c r="A254" s="2" t="s">
         <v>253</v>
       </c>
       <c r="B254" t="s">
@@ -4132,7 +4137,7 @@
       </c>
     </row>
     <row r="255" spans="1:2" ht="228" x14ac:dyDescent="0.45">
-      <c r="A255" s="3" t="s">
+      <c r="A255" s="2" t="s">
         <v>254</v>
       </c>
       <c r="B255" t="s">
@@ -4140,7 +4145,7 @@
       </c>
     </row>
     <row r="256" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A256" s="3" t="s">
+      <c r="A256" s="2" t="s">
         <v>255</v>
       </c>
       <c r="B256" t="s">
@@ -4148,7 +4153,7 @@
       </c>
     </row>
     <row r="257" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A257" s="3" t="s">
+      <c r="A257" s="2" t="s">
         <v>256</v>
       </c>
       <c r="B257" t="s">
@@ -4156,7 +4161,7 @@
       </c>
     </row>
     <row r="258" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A258" s="3" t="s">
+      <c r="A258" s="2" t="s">
         <v>257</v>
       </c>
       <c r="B258" t="s">
@@ -4164,7 +4169,7 @@
       </c>
     </row>
     <row r="259" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A259" s="3" t="s">
+      <c r="A259" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B259" t="s">
@@ -4172,7 +4177,7 @@
       </c>
     </row>
     <row r="260" spans="1:2" ht="228" x14ac:dyDescent="0.45">
-      <c r="A260" s="3" t="s">
+      <c r="A260" s="2" t="s">
         <v>259</v>
       </c>
       <c r="B260" t="s">
@@ -4180,7 +4185,7 @@
       </c>
     </row>
     <row r="261" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A261" s="3" t="s">
+      <c r="A261" s="2" t="s">
         <v>260</v>
       </c>
       <c r="B261" t="s">
@@ -4188,7 +4193,7 @@
       </c>
     </row>
     <row r="262" spans="1:2" ht="342" x14ac:dyDescent="0.45">
-      <c r="A262" s="3" t="s">
+      <c r="A262" s="2" t="s">
         <v>261</v>
       </c>
       <c r="B262" t="s">
@@ -4196,7 +4201,7 @@
       </c>
     </row>
     <row r="263" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A263" s="3" t="s">
+      <c r="A263" s="2" t="s">
         <v>262</v>
       </c>
       <c r="B263" t="s">
@@ -4204,7 +4209,7 @@
       </c>
     </row>
     <row r="264" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A264" s="3" t="s">
+      <c r="A264" s="2" t="s">
         <v>263</v>
       </c>
       <c r="B264" t="s">
@@ -4212,7 +4217,7 @@
       </c>
     </row>
     <row r="265" spans="1:2" ht="356.25" x14ac:dyDescent="0.45">
-      <c r="A265" s="3" t="s">
+      <c r="A265" s="2" t="s">
         <v>264</v>
       </c>
       <c r="B265" t="s">
@@ -4220,7 +4225,7 @@
       </c>
     </row>
     <row r="266" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A266" s="3" t="s">
+      <c r="A266" s="2" t="s">
         <v>265</v>
       </c>
       <c r="B266" t="s">
@@ -4228,7 +4233,7 @@
       </c>
     </row>
     <row r="267" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A267" s="3" t="s">
+      <c r="A267" s="2" t="s">
         <v>266</v>
       </c>
       <c r="B267" t="s">
@@ -4236,7 +4241,7 @@
       </c>
     </row>
     <row r="268" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A268" s="3" t="s">
+      <c r="A268" s="2" t="s">
         <v>267</v>
       </c>
       <c r="B268" t="s">
@@ -4244,7 +4249,7 @@
       </c>
     </row>
     <row r="269" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A269" s="3" t="s">
+      <c r="A269" s="2" t="s">
         <v>268</v>
       </c>
       <c r="B269" t="s">
@@ -4252,7 +4257,7 @@
       </c>
     </row>
     <row r="270" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A270" s="3" t="s">
+      <c r="A270" s="2" t="s">
         <v>269</v>
       </c>
       <c r="B270" t="s">
@@ -4260,7 +4265,7 @@
       </c>
     </row>
     <row r="271" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="A271" s="3" t="s">
+      <c r="A271" s="2" t="s">
         <v>270</v>
       </c>
       <c r="B271" t="s">
@@ -4268,7 +4273,7 @@
       </c>
     </row>
     <row r="272" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A272" s="3" t="s">
+      <c r="A272" s="2" t="s">
         <v>271</v>
       </c>
       <c r="B272" t="s">
@@ -4276,7 +4281,7 @@
       </c>
     </row>
     <row r="273" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A273" s="3" t="s">
+      <c r="A273" s="2" t="s">
         <v>272</v>
       </c>
       <c r="B273" t="s">
@@ -4284,7 +4289,7 @@
       </c>
     </row>
     <row r="274" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A274" s="3" t="s">
+      <c r="A274" s="2" t="s">
         <v>273</v>
       </c>
       <c r="B274" t="s">
@@ -4292,7 +4297,7 @@
       </c>
     </row>
     <row r="275" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A275" s="3" t="s">
+      <c r="A275" s="2" t="s">
         <v>274</v>
       </c>
       <c r="B275" t="s">
@@ -4300,7 +4305,7 @@
       </c>
     </row>
     <row r="276" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
-      <c r="A276" s="3" t="s">
+      <c r="A276" s="2" t="s">
         <v>275</v>
       </c>
       <c r="B276" t="s">
@@ -4308,7 +4313,7 @@
       </c>
     </row>
     <row r="277" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A277" s="3" t="s">
+      <c r="A277" s="2" t="s">
         <v>276</v>
       </c>
       <c r="B277" t="s">
@@ -4316,7 +4321,7 @@
       </c>
     </row>
     <row r="278" spans="1:2" ht="228" x14ac:dyDescent="0.45">
-      <c r="A278" s="3" t="s">
+      <c r="A278" s="2" t="s">
         <v>277</v>
       </c>
       <c r="B278" t="s">
@@ -4324,7 +4329,7 @@
       </c>
     </row>
     <row r="279" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A279" s="3" t="s">
+      <c r="A279" s="2" t="s">
         <v>278</v>
       </c>
       <c r="B279" t="s">
@@ -4332,7 +4337,7 @@
       </c>
     </row>
     <row r="280" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A280" s="3" t="s">
+      <c r="A280" s="2" t="s">
         <v>279</v>
       </c>
       <c r="B280" t="s">
@@ -4340,7 +4345,7 @@
       </c>
     </row>
     <row r="281" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
-      <c r="A281" s="3" t="s">
+      <c r="A281" s="2" t="s">
         <v>280</v>
       </c>
       <c r="B281" t="s">
@@ -4348,7 +4353,7 @@
       </c>
     </row>
     <row r="282" spans="1:2" ht="228" x14ac:dyDescent="0.45">
-      <c r="A282" s="3" t="s">
+      <c r="A282" s="2" t="s">
         <v>281</v>
       </c>
       <c r="B282" t="s">
@@ -4356,7 +4361,7 @@
       </c>
     </row>
     <row r="283" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A283" s="3" t="s">
+      <c r="A283" s="2" t="s">
         <v>282</v>
       </c>
       <c r="B283" t="s">
@@ -4364,7 +4369,7 @@
       </c>
     </row>
     <row r="284" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A284" s="3" t="s">
+      <c r="A284" s="2" t="s">
         <v>283</v>
       </c>
       <c r="B284" t="s">
@@ -4372,7 +4377,7 @@
       </c>
     </row>
     <row r="285" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
-      <c r="A285" s="3" t="s">
+      <c r="A285" s="2" t="s">
         <v>284</v>
       </c>
       <c r="B285" t="s">
@@ -4380,7 +4385,7 @@
       </c>
     </row>
     <row r="286" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A286" s="3" t="s">
+      <c r="A286" s="2" t="s">
         <v>285</v>
       </c>
       <c r="B286" t="s">
@@ -4388,7 +4393,7 @@
       </c>
     </row>
     <row r="287" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="A287" s="3" t="s">
+      <c r="A287" s="2" t="s">
         <v>286</v>
       </c>
       <c r="B287" t="s">
@@ -4396,7 +4401,7 @@
       </c>
     </row>
     <row r="288" spans="1:2" ht="228" x14ac:dyDescent="0.45">
-      <c r="A288" s="3" t="s">
+      <c r="A288" s="2" t="s">
         <v>287</v>
       </c>
       <c r="B288" t="s">
@@ -4404,7 +4409,7 @@
       </c>
     </row>
     <row r="289" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
-      <c r="A289" s="3" t="s">
+      <c r="A289" s="2" t="s">
         <v>288</v>
       </c>
       <c r="B289" t="s">
@@ -4412,7 +4417,7 @@
       </c>
     </row>
     <row r="290" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A290" s="3" t="s">
+      <c r="A290" s="2" t="s">
         <v>289</v>
       </c>
       <c r="B290" t="s">
@@ -4420,7 +4425,7 @@
       </c>
     </row>
     <row r="291" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
-      <c r="A291" s="3" t="s">
+      <c r="A291" s="2" t="s">
         <v>290</v>
       </c>
       <c r="B291" t="s">
@@ -4428,7 +4433,7 @@
       </c>
     </row>
     <row r="292" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A292" s="3" t="s">
+      <c r="A292" s="2" t="s">
         <v>291</v>
       </c>
       <c r="B292" t="s">
@@ -4436,7 +4441,7 @@
       </c>
     </row>
     <row r="293" spans="1:2" ht="342" x14ac:dyDescent="0.45">
-      <c r="A293" s="3" t="s">
+      <c r="A293" s="2" t="s">
         <v>292</v>
       </c>
       <c r="B293" t="s">
@@ -4449,7 +4454,7 @@
       </c>
     </row>
     <row r="295" spans="1:2" ht="285" x14ac:dyDescent="0.45">
-      <c r="A295" s="3" t="s">
+      <c r="A295" s="2" t="s">
         <v>293</v>
       </c>
       <c r="B295" t="s">
@@ -4457,7 +4462,7 @@
       </c>
     </row>
     <row r="296" spans="1:2" ht="171" x14ac:dyDescent="0.45">
-      <c r="A296" s="3" t="s">
+      <c r="A296" s="2" t="s">
         <v>294</v>
       </c>
       <c r="B296" t="s">
@@ -4465,7 +4470,7 @@
       </c>
     </row>
     <row r="297" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A297" s="3" t="s">
+      <c r="A297" s="2" t="s">
         <v>295</v>
       </c>
       <c r="B297" t="s">
@@ -4473,7 +4478,7 @@
       </c>
     </row>
     <row r="298" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A298" s="3" t="s">
+      <c r="A298" s="2" t="s">
         <v>296</v>
       </c>
       <c r="B298" t="s">
@@ -4481,7 +4486,7 @@
       </c>
     </row>
     <row r="299" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A299" s="3" t="s">
+      <c r="A299" s="2" t="s">
         <v>297</v>
       </c>
       <c r="B299" t="s">
@@ -4489,7 +4494,7 @@
       </c>
     </row>
     <row r="300" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A300" s="3" t="s">
+      <c r="A300" s="2" t="s">
         <v>298</v>
       </c>
       <c r="B300" t="s">
@@ -4497,7 +4502,7 @@
       </c>
     </row>
     <row r="301" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A301" s="3" t="s">
+      <c r="A301" s="2" t="s">
         <v>299</v>
       </c>
       <c r="B301" t="s">
@@ -4511,1014 +4516,1320 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A201"/>
+  <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="111.6640625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="15.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="B1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="B2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="B3" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="B4" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="B5" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="B6" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="B7" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="B8" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="B9" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="B10" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+      <c r="B11" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="B12" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="B13" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="B14" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="B15" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+      <c r="B16" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+      <c r="B17" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+      <c r="B18" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+      <c r="B19" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+      <c r="B20" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+      <c r="B21" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+      <c r="B22" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+      <c r="B23" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+      <c r="B24" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+      <c r="B25" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+      <c r="B26" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+      <c r="B27" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="2" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+      <c r="B28" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+      <c r="B29" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+      <c r="B30" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+      <c r="B31" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+      <c r="B32" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+      <c r="B33" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A34" s="2" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+      <c r="B34" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A35" s="2" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
+      <c r="B35" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+      <c r="B36" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A37" s="2" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
+      <c r="B37" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A38" s="2" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+      <c r="B38" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A39" s="2" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+      <c r="B39" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A40" s="2" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+      <c r="B40" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A41" s="2" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
+      <c r="B41" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A42" s="2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+      <c r="B42" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A43" s="2" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
+      <c r="B43" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A44" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
+      <c r="B44" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A45" s="2" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
+      <c r="B45" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A46" s="2" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+      <c r="B46" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A47" s="2" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
+      <c r="B47" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A48" s="2" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
+      <c r="B48" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A49" s="2" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+      <c r="B49" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A50" s="2" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+      <c r="B50" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A51" s="2" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+      <c r="B51" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A52" s="2" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+      <c r="B52" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A53" s="2" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+      <c r="B53" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A54" s="2" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
+      <c r="B54" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A55" s="2" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+      <c r="B55" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A56" s="2" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
+      <c r="B56" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A57" s="2" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
+      <c r="B57" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A58" s="2" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
+      <c r="B58" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A59" s="2" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
+      <c r="B59" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A60" s="2" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+      <c r="B60" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A61" s="2" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
+      <c r="B61" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A62" s="2" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
+      <c r="B62" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A63" s="2" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
+      <c r="B63" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A64" s="2" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
+      <c r="B64" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A65" s="2" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
+      <c r="B65" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A66" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
+      <c r="B66" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A67" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
+      <c r="B67" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A68" s="2" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
+      <c r="B68" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A69" s="2" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
+      <c r="B69" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A70" s="2" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
+      <c r="B70" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A71" s="2" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
+      <c r="B71" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A72" s="2" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
+      <c r="B72" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A73" s="2" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
+      <c r="B73" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A74" s="2" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
+      <c r="B74" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="A75" s="2" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
+      <c r="B75" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A76" s="2" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
+      <c r="B76" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A77" s="2" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
+      <c r="B77" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A78" s="2" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
+      <c r="B78" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A79" s="2" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
+      <c r="B79" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A80" s="2" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
+      <c r="B80" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A81" s="2" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
+      <c r="B81" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A82" s="2" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A83" t="s">
+      <c r="B82" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A83" s="2" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A84" t="s">
+      <c r="B83" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A84" s="2" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A85" t="s">
+      <c r="B84" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A85" s="2" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A86" t="s">
+      <c r="B85" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A86" s="2" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A87" t="s">
+      <c r="B86" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A87" s="2" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A88" t="s">
+      <c r="B87" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A88" s="2" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A89" t="s">
+      <c r="B88" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A89" s="2" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A90" t="s">
+      <c r="B89" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A90" s="2" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A91" t="s">
+      <c r="B90" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A91" s="2" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A92" t="s">
+      <c r="B91" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A92" s="2" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A93" t="s">
+      <c r="B92" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A93" s="2" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A94" t="s">
+      <c r="B93" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="A94" s="2" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A95" t="s">
+      <c r="B94" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A95" s="2" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A96" t="s">
+      <c r="B95" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A96" s="2" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A97" t="s">
+      <c r="B96" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A97" s="2" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A98" t="s">
+      <c r="B97" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A98" s="2" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A99" t="s">
+      <c r="B98" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A99" s="2" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A100" t="s">
+      <c r="B99" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A100" s="2" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A101" t="s">
+      <c r="B100" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A101" s="2" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A102" t="s">
+    <row r="102" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="A102" s="2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A103" t="s">
+    <row r="103" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A103" s="2" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A104" t="s">
+    <row r="104" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="A104" s="2" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A105" t="s">
+    <row r="105" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A105" s="2" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A106" t="s">
+    <row r="106" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A106" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A107" t="s">
+    <row r="107" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A107" s="2" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A108" t="s">
+    <row r="108" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A108" s="2" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A109" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A109" s="2" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A110" t="s">
+    <row r="110" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="A110" s="2" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A111" t="s">
+    <row r="111" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A111" s="2" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A112" t="s">
+    <row r="112" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A112" s="2" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A113" t="s">
+    <row r="113" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A113" s="2" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A114" t="s">
+    <row r="114" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A114" s="2" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A115" t="s">
+      <c r="A115" s="2" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A116" t="s">
+    <row r="116" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A116" s="2" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A117" t="s">
+    <row r="117" spans="1:1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A117" s="2" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A118" t="s">
+    <row r="118" spans="1:1" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A118" s="2" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A119" t="s">
+      <c r="A119" s="2" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A120" t="s">
+    <row r="120" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A120" s="2" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A121" t="s">
+      <c r="A121" s="2" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A122" t="s">
+      <c r="A122" s="2" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A123" t="s">
+      <c r="A123" s="2" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A124" t="s">
+      <c r="A124" s="2" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A125" t="s">
+      <c r="A125" s="2" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A126" t="s">
+      <c r="A126" s="2" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A127" t="s">
+      <c r="A127" s="2" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A128" t="s">
+      <c r="A128" s="2" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A129" t="s">
+    <row r="129" spans="1:1" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A129" s="2" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A130" t="s">
+      <c r="A130" s="2" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A131" t="s">
+    <row r="131" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A131" s="2" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A132" t="s">
+      <c r="A132" s="2" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A133" t="s">
+    <row r="133" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A133" s="2" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A134" t="s">
+      <c r="A134" s="2" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A135" t="s">
+      <c r="A135" s="2" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A136" t="s">
+      <c r="A136" s="2" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A137" t="s">
+    <row r="137" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A137" s="2" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A138" t="s">
+      <c r="A138" s="2" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A139" t="s">
+      <c r="A139" s="2" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A140" t="s">
+      <c r="A140" s="2" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A141" t="s">
+      <c r="A141" s="2" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A142" t="s">
+    <row r="142" spans="1:1" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A142" s="2" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A143" t="s">
+    <row r="143" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A143" s="2" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A144" t="s">
+    <row r="144" spans="1:1" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A144" s="2" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A145" t="s">
+      <c r="A145" s="2" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A146" t="s">
+    <row r="146" spans="1:1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A146" s="2" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A147" t="s">
+      <c r="A147" s="2" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A148" t="s">
+      <c r="A148" s="2" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A149" t="s">
+    <row r="149" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A149" s="2" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A150" t="s">
+    <row r="150" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A150" s="2" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A151" t="s">
+    <row r="151" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A151" s="2" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A152" t="s">
+      <c r="A152" s="2" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A153" t="s">
+    <row r="153" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A153" s="2" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A154" t="s">
+      <c r="A154" s="2" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A155" t="s">
+      <c r="A155" s="2" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A156" t="s">
+      <c r="A156" s="2" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A157" t="s">
+      <c r="A157" s="2" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A158" t="s">
+    <row r="158" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A158" s="2" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A159" t="s">
+      <c r="A159" s="2" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A160" t="s">
+    <row r="160" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A160" s="2" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A161" t="s">
+    <row r="161" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A161" s="2" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A162" t="s">
+    <row r="162" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A162" s="2" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A163" t="s">
+      <c r="A163" s="2" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A164" t="s">
+    <row r="164" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A164" s="2" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A165" t="s">
+      <c r="A165" s="2" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A166" t="s">
+    <row r="166" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A166" s="2" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A167" t="s">
+      <c r="A167" s="2" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A168" t="s">
+    <row r="168" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A168" s="2" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A169" t="s">
+    <row r="169" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A169" s="2" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A170" t="s">
+    <row r="170" spans="1:1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A170" s="2" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A171" t="s">
+    <row r="171" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A171" s="2" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A172" t="s">
+    <row r="172" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A172" s="2" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A173" t="s">
+      <c r="A173" s="2" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A174" t="s">
+      <c r="A174" s="2" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A175" t="s">
+      <c r="A175" s="2" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A176" t="s">
+    <row r="176" spans="1:1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A176" s="2" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A177" t="s">
+      <c r="A177" s="2" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A178" t="s">
+    <row r="178" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A178" s="2" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A179" t="s">
+    <row r="179" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A179" s="2" t="s">
         <v>477</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A180" t="s">
+      <c r="A180" s="2" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A181" t="s">
+    <row r="181" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A181" s="2" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A182" t="s">
+    <row r="182" spans="1:1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A182" s="2" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A183" t="s">
+    <row r="183" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A183" s="2" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A184" t="s">
+    <row r="184" spans="1:1" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A184" s="2" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A185" t="s">
+      <c r="A185" s="2" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A186" t="s">
+    <row r="186" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A186" s="2" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A187" t="s">
+      <c r="A187" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A188" t="s">
+    <row r="188" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A188" s="2" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A189" t="s">
+      <c r="A189" s="2" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A190" t="s">
+      <c r="A190" s="2" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A191" t="s">
+      <c r="A191" s="2" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A192" t="s">
+    <row r="192" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A192" s="2" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A193" t="s">
+    <row r="193" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A193" s="2" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A194" t="s">
+    <row r="194" spans="1:1" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A194" s="2" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A195" t="s">
+      <c r="A195" s="2" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A196" t="s">
+      <c r="A196" s="2" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A197" t="s">
+      <c r="A197" s="2" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A198" t="s">
+    <row r="198" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A198" s="2" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A199" t="s">
+      <c r="A199" s="2" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A200" t="s">
+      <c r="A200" s="2" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A201" t="s">
+      <c r="A201" s="2" t="s">
         <v>499</v>
       </c>
     </row>

</xml_diff>

<commit_message>
avaliei as 100 do teste
</commit_message>
<xml_diff>
--- a/SPTrans.xlsx
+++ b/SPTrans.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crazy\Documents\Projetos\P2_CD19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\André Luis Silva Lop\Documents\INSPER\twitter\P2_CD19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A834ABD-4247-4580-92F9-2ADE99237AC8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12A4726-DF05-479D-AC8A-5A7B76790A8D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
     <sheet name="Teste" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="502">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1688,9 +1687,6 @@
   </si>
   <si>
     <t>I</t>
-  </si>
-  <si>
-    <t>Classificacao</t>
   </si>
 </sst>
 </file>
@@ -2097,25 +2093,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="G150" sqref="G150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2123,7 +2115,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2131,7 +2123,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2139,7 +2131,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2147,7 +2139,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -2155,7 +2147,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2163,7 +2155,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2171,7 +2163,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2179,7 +2171,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -2187,7 +2179,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -2195,7 +2187,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="285" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -2203,7 +2195,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -2211,7 +2203,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -2219,7 +2211,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -2227,7 +2219,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -2235,7 +2227,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="356.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" ht="360" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -2243,7 +2235,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -2251,7 +2243,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -2259,7 +2251,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="228" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -2267,7 +2259,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -2275,7 +2267,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" ht="360" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2283,7 +2275,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -2291,7 +2283,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -2299,7 +2291,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -2307,7 +2299,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="342" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -2315,7 +2307,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -2323,7 +2315,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -2331,7 +2323,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -2339,7 +2331,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -2347,7 +2339,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -2355,7 +2347,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -2363,7 +2355,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -2371,7 +2363,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -2379,7 +2371,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -2387,7 +2379,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -2395,7 +2387,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -2403,7 +2395,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="228" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -2411,7 +2403,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="285" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -2419,7 +2411,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
@@ -2427,7 +2419,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="228" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
@@ -2435,7 +2427,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
@@ -2443,7 +2435,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="285" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
@@ -2451,7 +2443,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
@@ -2459,7 +2451,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
@@ -2467,7 +2459,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
@@ -2475,7 +2467,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -2483,7 +2475,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
@@ -2491,7 +2483,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
@@ -2499,7 +2491,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
@@ -2507,7 +2499,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="342" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
@@ -2515,7 +2507,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -2523,7 +2515,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
@@ -2531,7 +2523,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
@@ -2539,7 +2531,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
@@ -2547,7 +2539,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
@@ -2555,7 +2547,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
@@ -2563,7 +2555,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
@@ -2571,7 +2563,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
@@ -2579,7 +2571,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
@@ -2587,7 +2579,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
@@ -2595,7 +2587,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
@@ -2603,7 +2595,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="285" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
@@ -2611,7 +2603,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
@@ -2619,7 +2611,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
@@ -2627,7 +2619,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>65</v>
       </c>
@@ -2635,7 +2627,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
@@ -2643,7 +2635,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="242.25" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>67</v>
       </c>
@@ -2651,7 +2643,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>68</v>
       </c>
@@ -2659,7 +2651,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
@@ -2667,7 +2659,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
@@ -2675,7 +2667,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="228" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>71</v>
       </c>
@@ -2683,7 +2675,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
@@ -2691,7 +2683,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="228" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>73</v>
       </c>
@@ -2699,7 +2691,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>74</v>
       </c>
@@ -2707,7 +2699,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
@@ -2715,7 +2707,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
@@ -2723,7 +2715,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>77</v>
       </c>
@@ -2731,7 +2723,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -2739,7 +2731,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="285" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
@@ -2747,7 +2739,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
@@ -2755,7 +2747,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:2" ht="360" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>81</v>
       </c>
@@ -2763,7 +2755,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>82</v>
       </c>
@@ -2771,7 +2763,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>83</v>
       </c>
@@ -2779,7 +2771,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>84</v>
       </c>
@@ -2787,7 +2779,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>85</v>
       </c>
@@ -2795,7 +2787,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>86</v>
       </c>
@@ -2803,7 +2795,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>87</v>
       </c>
@@ -2811,7 +2803,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="342" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:2" ht="360" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>88</v>
       </c>
@@ -2819,7 +2811,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>89</v>
       </c>
@@ -2827,7 +2819,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>90</v>
       </c>
@@ -2835,7 +2827,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="356.25" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
@@ -2843,7 +2835,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>92</v>
       </c>
@@ -2851,7 +2843,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>93</v>
       </c>
@@ -2859,7 +2851,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>94</v>
       </c>
@@ -2867,7 +2859,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>95</v>
       </c>
@@ -2875,7 +2867,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
@@ -2883,7 +2875,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="384.75" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>97</v>
       </c>
@@ -2891,7 +2883,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>98</v>
       </c>
@@ -2899,7 +2891,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="342" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2" ht="360" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>99</v>
       </c>
@@ -2907,7 +2899,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="285" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
@@ -2915,7 +2907,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>101</v>
       </c>
@@ -2923,7 +2915,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>102</v>
       </c>
@@ -2931,7 +2923,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="342" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:2" ht="360" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>103</v>
       </c>
@@ -2939,7 +2931,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>104</v>
       </c>
@@ -2947,7 +2939,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>105</v>
       </c>
@@ -2955,7 +2947,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="342" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>106</v>
       </c>
@@ -2963,7 +2955,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>107</v>
       </c>
@@ -2971,7 +2963,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>108</v>
       </c>
@@ -2979,7 +2971,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>109</v>
       </c>
@@ -2987,7 +2979,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="228" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>110</v>
       </c>
@@ -2995,7 +2987,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>111</v>
       </c>
@@ -3003,7 +2995,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>112</v>
       </c>
@@ -3011,7 +3003,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>113</v>
       </c>
@@ -3019,7 +3011,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>114</v>
       </c>
@@ -3027,7 +3019,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="228" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>115</v>
       </c>
@@ -3035,7 +3027,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>116</v>
       </c>
@@ -3043,7 +3035,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>117</v>
       </c>
@@ -3051,7 +3043,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>118</v>
       </c>
@@ -3059,7 +3051,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>119</v>
       </c>
@@ -3067,7 +3059,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>120</v>
       </c>
@@ -3075,7 +3067,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>121</v>
       </c>
@@ -3083,7 +3075,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>122</v>
       </c>
@@ -3091,7 +3083,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>123</v>
       </c>
@@ -3099,7 +3091,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>124</v>
       </c>
@@ -3107,7 +3099,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>125</v>
       </c>
@@ -3115,7 +3107,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>126</v>
       </c>
@@ -3123,7 +3115,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>127</v>
       </c>
@@ -3131,7 +3123,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>128</v>
       </c>
@@ -3139,7 +3131,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>129</v>
       </c>
@@ -3147,7 +3139,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="370.5" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>130</v>
       </c>
@@ -3155,7 +3147,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>131</v>
       </c>
@@ -3163,7 +3155,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>132</v>
       </c>
@@ -3171,7 +3163,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>133</v>
       </c>
@@ -3179,7 +3171,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>134</v>
       </c>
@@ -3187,7 +3179,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>135</v>
       </c>
@@ -3195,7 +3187,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>136</v>
       </c>
@@ -3203,7 +3195,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>137</v>
       </c>
@@ -3211,7 +3203,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="356.25" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:2" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>138</v>
       </c>
@@ -3219,7 +3211,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>139</v>
       </c>
@@ -3227,7 +3219,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>140</v>
       </c>
@@ -3235,7 +3227,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>141</v>
       </c>
@@ -3243,7 +3235,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>142</v>
       </c>
@@ -3251,7 +3243,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>143</v>
       </c>
@@ -3259,7 +3251,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>144</v>
       </c>
@@ -3267,7 +3259,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>145</v>
       </c>
@@ -3275,7 +3267,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>146</v>
       </c>
@@ -3283,7 +3275,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>147</v>
       </c>
@@ -3291,7 +3283,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>148</v>
       </c>
@@ -3299,7 +3291,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>149</v>
       </c>
@@ -3307,1206 +3299,754 @@
         <v>500</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B151" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    </row>
+    <row r="152" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B152" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="153" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B153" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    </row>
+    <row r="154" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B154" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="155" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B155" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="156" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B156" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    </row>
+    <row r="157" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B157" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    </row>
+    <row r="158" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B158" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="159" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B159" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="160" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B160" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="161" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B161" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="162" spans="1:1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B162" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="163" spans="1:1" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B163" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    </row>
+    <row r="164" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B164" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="165" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B165" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="166" spans="1:1" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B166" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="167" spans="1:1" ht="288" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B167" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    </row>
+    <row r="168" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B168" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    </row>
+    <row r="169" spans="1:1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B169" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="342" x14ac:dyDescent="0.45">
+    </row>
+    <row r="170" spans="1:1" ht="360" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B170" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="171" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B171" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="172" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B172" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="173" spans="1:1" ht="144" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B173" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="174" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B174" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="175" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B175" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="176" spans="1:1" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B176" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="177" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B177" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="178" spans="1:1" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B178" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    </row>
+    <row r="179" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B179" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="370.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="180" spans="1:1" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B180" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="181" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B181" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="182" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B182" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="183" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B183" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    </row>
+    <row r="184" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B184" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    </row>
+    <row r="185" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B185" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="186" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B186" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="187" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B187" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="188" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B188" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="189" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B189" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="190" spans="1:1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B190" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="191" spans="1:1" ht="144" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B191" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="192" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B192" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" ht="242.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="193" spans="1:1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B193" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="194" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B194" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="195" spans="1:1" ht="144" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B195" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="196" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B196" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="197" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B197" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="198" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B198" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="199" spans="1:1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B199" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="200" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B200" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="201" spans="1:1" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B201" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    </row>
+    <row r="202" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B202" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    </row>
+    <row r="203" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B203" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="204" spans="1:1" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B204" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    </row>
+    <row r="205" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B205" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="206" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B206" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="207" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B208" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" ht="242.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="209" spans="1:1" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B209" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" ht="342" x14ac:dyDescent="0.45">
+    </row>
+    <row r="210" spans="1:1" ht="360" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B210" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="211" spans="1:1" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B211" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="212" spans="1:1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B212" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="213" spans="1:1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B213" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" ht="242.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="214" spans="1:1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B214" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="215" spans="1:1" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B215" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="216" spans="1:1" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B216" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="217" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B217" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    </row>
+    <row r="218" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B218" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="219" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B219" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="220" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B220" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="342" x14ac:dyDescent="0.45">
+    </row>
+    <row r="221" spans="1:1" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B221" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    </row>
+    <row r="222" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B222" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="223" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B223" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    </row>
+    <row r="224" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B224" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="225" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B225" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="226" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B226" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="227" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B227" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="228" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B228" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    </row>
+    <row r="229" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B229" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    </row>
+    <row r="230" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B230" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="231" spans="1:1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="B231" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    </row>
+    <row r="232" spans="1:1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B232" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="233" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B233" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="234" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B234" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="235" spans="1:1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B235" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="236" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B236" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" ht="242.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="237" spans="1:1" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B237" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="238" spans="1:1" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B238" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="239" spans="1:1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B239" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="240" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B240" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="241" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B241" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="242" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B242" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="243" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B243" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="244" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B244" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    </row>
+    <row r="245" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B245" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="246" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B246" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="247" spans="1:1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B247" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="248" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B248" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="249" spans="1:1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B249" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="250" spans="1:1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="B250" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="251" spans="1:1" ht="288" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B251" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="252" spans="1:1" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B252" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="253" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B253" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="254" spans="1:1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B254" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" ht="228" x14ac:dyDescent="0.45">
+    </row>
+    <row r="255" spans="1:1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B255" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="256" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B256" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="257" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B257" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="258" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B258" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="259" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B259" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" ht="228" x14ac:dyDescent="0.45">
+    </row>
+    <row r="260" spans="1:1" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B260" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    </row>
+    <row r="261" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B261" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" ht="342" x14ac:dyDescent="0.45">
+    </row>
+    <row r="262" spans="1:1" ht="360" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B262" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="263" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B263" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="264" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B264" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" ht="356.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="265" spans="1:1" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B265" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="266" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B266" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    </row>
+    <row r="267" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B267" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="268" spans="1:1" ht="144" x14ac:dyDescent="0.3">
       <c r="A268" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B268" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="269" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A269" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B269" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="270" spans="1:1" ht="144" x14ac:dyDescent="0.3">
       <c r="A270" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B270" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="271" spans="1:1" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A271" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B271" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="272" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A272" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B272" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="273" spans="1:1" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A273" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B273" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="274" spans="1:1" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A274" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B274" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="275" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B275" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="276" spans="1:1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B276" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="277" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A277" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B277" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" ht="228" x14ac:dyDescent="0.45">
+    </row>
+    <row r="278" spans="1:1" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A278" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B278" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="279" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A279" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B279" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    </row>
+    <row r="280" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A280" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B280" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" ht="299.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="281" spans="1:1" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A281" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B281" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" ht="228" x14ac:dyDescent="0.45">
+    </row>
+    <row r="282" spans="1:1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A282" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B282" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="283" spans="1:1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A283" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B283" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="284" spans="1:1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A284" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B284" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="285" spans="1:1" ht="288" x14ac:dyDescent="0.3">
       <c r="A285" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B285" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" ht="256.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="286" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A286" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B286" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="287" spans="1:1" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A287" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B287" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" ht="228" x14ac:dyDescent="0.45">
+    </row>
+    <row r="288" spans="1:1" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A288" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B288" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="289" spans="1:1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A289" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B289" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="290" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A290" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="B290" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="291" spans="1:1" ht="288" x14ac:dyDescent="0.3">
       <c r="A291" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B291" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="292" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A292" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B292" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" ht="342" x14ac:dyDescent="0.45">
+    </row>
+    <row r="293" spans="1:1" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A293" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B293" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B294" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2" ht="285" x14ac:dyDescent="0.45">
+    </row>
+    <row r="295" spans="1:1" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A295" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B295" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" ht="171" x14ac:dyDescent="0.45">
+    </row>
+    <row r="296" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A296" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B296" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="297" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A297" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B297" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="298" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A298" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B298" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="299" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A299" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B299" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="300" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="300" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A300" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B300" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="301" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="301" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A301" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="B301" t="s">
-        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -4518,25 +4058,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="111.6640625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>301</v>
       </c>
@@ -4544,7 +4080,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>302</v>
       </c>
@@ -4552,7 +4088,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>303</v>
       </c>
@@ -4560,15 +4096,15 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>304</v>
       </c>
       <c r="B5" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>305</v>
       </c>
@@ -4576,7 +4112,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>306</v>
       </c>
@@ -4584,7 +4120,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>307</v>
       </c>
@@ -4592,7 +4128,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>308</v>
       </c>
@@ -4600,7 +4136,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>309</v>
       </c>
@@ -4608,7 +4144,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>310</v>
       </c>
@@ -4616,7 +4152,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>311</v>
       </c>
@@ -4624,7 +4160,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>312</v>
       </c>
@@ -4632,15 +4168,15 @@
         <v>501</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>313</v>
       </c>
       <c r="B14" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>314</v>
       </c>
@@ -4648,23 +4184,23 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>315</v>
       </c>
       <c r="B16" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>316</v>
       </c>
       <c r="B17" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>317</v>
       </c>
@@ -4672,15 +4208,12 @@
         <v>501</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B19" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>319</v>
       </c>
@@ -4688,7 +4221,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>320</v>
       </c>
@@ -4696,7 +4229,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>321</v>
       </c>
@@ -4704,7 +4237,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>322</v>
       </c>
@@ -4712,7 +4245,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>323</v>
       </c>
@@ -4720,31 +4253,31 @@
         <v>501</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>324</v>
       </c>
       <c r="B25" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>325</v>
       </c>
       <c r="B26" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>326</v>
       </c>
       <c r="B27" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>327</v>
       </c>
@@ -4752,7 +4285,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>328</v>
       </c>
@@ -4760,15 +4293,15 @@
         <v>500</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>329</v>
       </c>
       <c r="B30" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>330</v>
       </c>
@@ -4776,7 +4309,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>331</v>
       </c>
@@ -4784,7 +4317,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>332</v>
       </c>
@@ -4792,7 +4325,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>333</v>
       </c>
@@ -4800,7 +4333,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>334</v>
       </c>
@@ -4808,15 +4341,12 @@
         <v>501</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B36" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="37" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>336</v>
       </c>
@@ -4824,15 +4354,15 @@
         <v>501</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>337</v>
       </c>
       <c r="B38" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>338</v>
       </c>
@@ -4840,7 +4370,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>339</v>
       </c>
@@ -4848,7 +4378,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>340</v>
       </c>
@@ -4856,15 +4386,15 @@
         <v>501</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>341</v>
       </c>
       <c r="B42" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>342</v>
       </c>
@@ -4872,7 +4402,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>343</v>
       </c>
@@ -4880,7 +4410,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>344</v>
       </c>
@@ -4888,15 +4418,15 @@
         <v>501</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>345</v>
       </c>
       <c r="B46" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>346</v>
       </c>
@@ -4904,7 +4434,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>347</v>
       </c>
@@ -4912,15 +4442,15 @@
         <v>500</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>348</v>
       </c>
       <c r="B49" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>349</v>
       </c>
@@ -4928,7 +4458,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>350</v>
       </c>
@@ -4936,7 +4466,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>351</v>
       </c>
@@ -4944,7 +4474,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>352</v>
       </c>
@@ -4952,7 +4482,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>353</v>
       </c>
@@ -4960,7 +4490,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>354</v>
       </c>
@@ -4968,7 +4498,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>355</v>
       </c>
@@ -4976,7 +4506,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>356</v>
       </c>
@@ -4984,15 +4514,15 @@
         <v>500</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>357</v>
       </c>
       <c r="B58" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>358</v>
       </c>
@@ -5000,7 +4530,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>359</v>
       </c>
@@ -5008,7 +4538,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>360</v>
       </c>
@@ -5016,7 +4546,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>361</v>
       </c>
@@ -5024,7 +4554,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>362</v>
       </c>
@@ -5032,7 +4562,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>363</v>
       </c>
@@ -5040,7 +4570,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>364</v>
       </c>
@@ -5048,7 +4578,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>365</v>
       </c>
@@ -5056,7 +4586,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>366</v>
       </c>
@@ -5064,7 +4594,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>367</v>
       </c>
@@ -5072,7 +4602,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>368</v>
       </c>
@@ -5080,7 +4610,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>369</v>
       </c>
@@ -5088,15 +4618,15 @@
         <v>501</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>370</v>
       </c>
       <c r="B71" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="360" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>371</v>
       </c>
@@ -5104,7 +4634,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>372</v>
       </c>
@@ -5112,7 +4642,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>373</v>
       </c>
@@ -5120,7 +4650,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>374</v>
       </c>
@@ -5128,7 +4658,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>375</v>
       </c>
@@ -5136,7 +4666,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>376</v>
       </c>
@@ -5144,7 +4674,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>377</v>
       </c>
@@ -5152,7 +4682,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>378</v>
       </c>
@@ -5160,7 +4690,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>379</v>
       </c>
@@ -5168,15 +4698,15 @@
         <v>501</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>380</v>
       </c>
       <c r="B81" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>381</v>
       </c>
@@ -5184,7 +4714,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>382</v>
       </c>
@@ -5192,15 +4722,15 @@
         <v>501</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>383</v>
       </c>
       <c r="B84" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>384</v>
       </c>
@@ -5208,7 +4738,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:2" ht="360" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>385</v>
       </c>
@@ -5216,7 +4746,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>386</v>
       </c>
@@ -5224,15 +4754,15 @@
         <v>501</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>387</v>
       </c>
       <c r="B88" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>388</v>
       </c>
@@ -5240,7 +4770,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>389</v>
       </c>
@@ -5248,15 +4778,15 @@
         <v>501</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>390</v>
       </c>
       <c r="B91" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>391</v>
       </c>
@@ -5264,15 +4794,15 @@
         <v>501</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>392</v>
       </c>
       <c r="B93" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>393</v>
       </c>
@@ -5280,7 +4810,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>394</v>
       </c>
@@ -5288,7 +4818,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>395</v>
       </c>
@@ -5296,7 +4826,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>396</v>
       </c>
@@ -5304,7 +4834,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>397</v>
       </c>
@@ -5312,7 +4842,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>398</v>
       </c>
@@ -5320,7 +4850,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>399</v>
       </c>
@@ -5328,507 +4858,507 @@
         <v>501</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:2" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:1" ht="360" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="57" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:1" ht="216" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="129" spans="1:1" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="131" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="133" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="137" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:1" ht="360" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:1" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="142" spans="1:1" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="143" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:1" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="144" spans="1:1" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="146" spans="1:1" ht="57" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="149" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:1" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="150" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:1" ht="288" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="151" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="153" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:1" ht="216" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="158" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="160" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="161" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="162" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:1" ht="144" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="164" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="166" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:1" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="168" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="169" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="170" spans="1:1" ht="57" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:1" ht="288" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="171" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:1" ht="216" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="172" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:1" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:1" ht="216" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:1" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="176" spans="1:1" ht="57" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:1" ht="360" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="178" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:1" ht="360" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="179" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="181" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:1" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="182" spans="1:1" ht="57" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:1" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="183" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="184" spans="1:1" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="186" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:1" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="188" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="192" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="193" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="194" spans="1:1" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:1" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:1" ht="216" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="198" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>499</v>
       </c>

</xml_diff>